<commit_message>
Last update before merging with NLP tools
</commit_message>
<xml_diff>
--- a/data/filtered_data.xlsx
+++ b/data/filtered_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ualbertaca-my.sharepoint.com/personal/hqiu1_ualberta_ca/Documents/Lab (Taufik)/NeuromodulationNLP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ualbertaca-my.sharepoint.com/personal/hqiu1_ualberta_ca/Documents/Lab (Taufik)/NeuromodulationNLP/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="11_E5167EC865112FE342170B88F3D9EF81502EC241" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="14400" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1447,8 +1447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>

</xml_diff>